<commit_message>
DBMS-35. Master Chado DW: Stock Centers Dataflow
https://jira.araport.org/browse/DBMS-35

1. Code for dbxref
</commit_message>
<xml_diff>
--- a/docs/tairchadodataflow.xlsx
+++ b/docs/tairchadodataflow.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1720" windowWidth="26340" windowHeight="15820" activeTab="2"/>
+    <workbookView xWindow="1160" yWindow="0" windowWidth="29700" windowHeight="19260" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Source - TAIR Entities" sheetId="2" r:id="rId1"/>
     <sheet name="Destination - CHADO Entities" sheetId="3" r:id="rId2"/>
-    <sheet name="Source To Target Transformation" sheetId="4" r:id="rId3"/>
+    <sheet name="SrcToTarget- General Module" sheetId="5" r:id="rId3"/>
+    <sheet name="SrcToTarget - Stock Types" sheetId="4" r:id="rId4"/>
+    <sheet name="Connections" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="134">
   <si>
     <t>Entity Name</t>
   </si>
@@ -233,9 +235,6 @@
     <t>Data Flow Steps</t>
   </si>
   <si>
-    <t>Load Stock Types</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -278,42 +277,24 @@
     <t>SQL Statement</t>
   </si>
   <si>
-    <t>CVTERM</t>
-  </si>
-  <si>
     <t>Precondidtion</t>
   </si>
   <si>
-    <t>Identify reference for the stock_type</t>
-  </si>
-  <si>
     <t>Bootstrap</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>If not exists, create one.</t>
-  </si>
-  <si>
     <t>CV</t>
   </si>
   <si>
     <t>The reference to the controlled vocabulary that corresponds to the STOCK_TYPE must exist before loading STOCK TYPE records from TAIR.</t>
   </si>
   <si>
-    <t>CV table has attached sequence to the cv_id column. We don't have to worry about primary key creation.</t>
-  </si>
-  <si>
-    <t>INSERT INTO CV (NAME, DEFINITION) VALUES ('stock_type', 'Contains a list of types for stocks.');</t>
-  </si>
-  <si>
     <t>Bootstrap SQL</t>
   </si>
   <si>
-    <t>ALTER DEFAULT PRIVILEGES IN SCHEMA public GRANT SELECT ON TABLES TO tripal2;</t>
-  </si>
-  <si>
     <t xml:space="preserve">            'SELECT cv_id </t>
   </si>
   <si>
@@ -326,13 +307,124 @@
     <t>SELECT cv.* FROM dblink('dbname=tair_tables host=pgsql-lan-dev user=tripal password=iPv8yR44s',</t>
   </si>
   <si>
-    <t>select * from CV where name = 'stock_type'</t>
-  </si>
-  <si>
-    <t>SELECT * FROM dbxref where accession='local:null';</t>
-  </si>
-  <si>
-    <t>dbxref must exist</t>
+    <t>Step Description</t>
+  </si>
+  <si>
+    <t>Each Stock Type Should have references in DB, DBXREF, CV &amp; CV_TERM tables</t>
+  </si>
+  <si>
+    <t>Populating General Module - External References</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>Create record in the the cross-refence table DBXREF to link TAIR Stock Objects by term back to the source database.</t>
+  </si>
+  <si>
+    <t>Create DBXREF record: "stock_type"</t>
+  </si>
+  <si>
+    <t>Match by accession field: "stock_type"</t>
+  </si>
+  <si>
+    <t>dbxref_stock_type.sql</t>
+  </si>
+  <si>
+    <t>Match by name field: "stock_type"</t>
+  </si>
+  <si>
+    <t>Matching By</t>
+  </si>
+  <si>
+    <t>Matching Value</t>
+  </si>
+  <si>
+    <t>accession</t>
+  </si>
+  <si>
+    <t>stock_type</t>
+  </si>
+  <si>
+    <t>Create DBXREF record: "stock_availability"</t>
+  </si>
+  <si>
+    <t>Match by accession field: "stock_availability"</t>
+  </si>
+  <si>
+    <t>stock_availability</t>
+  </si>
+  <si>
+    <t>dbxref_stock_availability.sql</t>
+  </si>
+  <si>
+    <t>Create CV record for key value "stock_type"</t>
+  </si>
+  <si>
+    <t>Match by name field: "stock_availability"</t>
+  </si>
+  <si>
+    <t>Populating General Module: Stock Types &amp; Stock Availability Types</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>dbxref_cv_stock_type.sql</t>
+  </si>
+  <si>
+    <t>Create CV record for "stock_availability"</t>
+  </si>
+  <si>
+    <t>The reference to the controlled vocabulary that corresponds to the STOCK_AVAILABILITY_TYPE must exist before loading STOCK TYPE records from TAIR.</t>
+  </si>
+  <si>
+    <t>dbxref_cv_stock_availability.sql</t>
+  </si>
+  <si>
+    <t>SQL Statement/Script</t>
+  </si>
+  <si>
+    <t>DBXREF</t>
+  </si>
+  <si>
+    <t>TAIR Stock</t>
+  </si>
+  <si>
+    <t>Matching</t>
+  </si>
+  <si>
+    <t>Match by name field: "TAIR Stock"</t>
+  </si>
+  <si>
+    <t>Result:db_id that represents tair_stock_db_id</t>
+  </si>
+  <si>
+    <t>Create TAIR External Databases in the DB Table</t>
+  </si>
+  <si>
+    <t>Populate DB &amp; DBXREF Tables with references to the TAIR Stock Database Objects. These database objects will be used by individual stocks and its components.</t>
+  </si>
+  <si>
+    <t>Match by tair_stock_db_id, and database tair_object_id</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>db_init.sql</t>
+  </si>
+  <si>
+    <t>This can deferred until actual object creation</t>
+  </si>
+  <si>
+    <t>GERMPLAZMS</t>
+  </si>
+  <si>
+    <t>etc</t>
   </si>
 </sst>
 </file>
@@ -406,7 +498,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -430,8 +522,42 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -439,8 +565,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -452,6 +581,23 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -463,6 +609,23 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1220,187 +1383,479 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor rgb="FF0070C0"/>
+    <tabColor rgb="FF131D5C"/>
   </sheetPr>
-  <dimension ref="A2:I22"/>
+  <dimension ref="A4:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="23.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="41.83203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="21" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="19" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="2" width="18.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" style="2" customWidth="1"/>
+    <col min="4" max="7" width="23.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="27.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="21" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="19" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
-      <c r="B2" s="2" t="s">
+    <row r="4" spans="1:12" ht="19" customHeight="1">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="6" spans="1:12" ht="17" customHeight="1">
+      <c r="B6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="43" customHeight="1">
+      <c r="B7" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" ht="26">
+      <c r="C10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" ht="72" customHeight="1">
+      <c r="C11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="E16" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4">
+      <c r="C19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4">
+      <c r="C20" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4">
+      <c r="C21" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A2:M25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="2" width="18.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="23.33203125" style="2" customWidth="1"/>
+    <col min="6" max="7" width="14.83203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="41.83203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="19" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11">
+      <c r="C2" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:11">
+      <c r="C6" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="B6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:11">
+      <c r="C7" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="B7" s="2" t="s">
+      <c r="D7" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="14">
+      <c r="C8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D8" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="14">
-      <c r="B8" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D8"/>
       <c r="E8"/>
-    </row>
-    <row r="11" spans="1:9" ht="19" customHeight="1">
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+    </row>
+    <row r="11" spans="1:11" ht="19" customHeight="1">
       <c r="A11" s="1">
         <v>1</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-    </row>
-    <row r="13" spans="1:9" ht="17" customHeight="1">
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="13" spans="1:11" ht="35" customHeight="1">
       <c r="B13" s="1" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="43" customHeight="1">
+      <c r="B14" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:13" ht="26">
+      <c r="D17" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="1" t="s">
+      <c r="K17" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="26">
+      <c r="A18" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="39">
+      <c r="A19" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" ht="117">
-      <c r="C16" s="2" t="s">
+      <c r="I19" s="4"/>
+      <c r="J19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="1:13" ht="72" customHeight="1">
+      <c r="A20" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:13" ht="195">
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="M22" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="39">
+      <c r="I23" s="4"/>
+      <c r="M23" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="39">
+      <c r="I24" s="4"/>
+      <c r="M24" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E16" s="4" t="s">
+    </row>
+    <row r="25" spans="1:13" ht="39">
+      <c r="I25" s="4"/>
+      <c r="M25" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" ht="72" customHeight="1">
-      <c r="D17" s="4"/>
-      <c r="E17" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="2:9">
-      <c r="D18" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="2:9" ht="65">
-      <c r="D19" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9">
-      <c r="F20" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9">
-      <c r="B21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9">
-      <c r="F22" s="4" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1412,4 +1867,74 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor rgb="FF008000"/>
+  </sheetPr>
+  <dimension ref="A2:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="2" spans="1:6" s="2" customFormat="1" ht="13"/>
+    <row r="3" spans="1:6" s="2" customFormat="1" ht="13"/>
+    <row r="4" spans="1:6" s="2" customFormat="1" ht="13">
+      <c r="A4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="13">
+      <c r="A5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="2" customFormat="1" ht="13">
+      <c r="C6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="2" customFormat="1" ht="13">
+      <c r="C7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="2" customFormat="1">
+      <c r="C8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8"/>
+      <c r="F8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>